<commit_message>
* enable sheet protection * set unlocked cells * hide sheet tab and toolbar
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/vendor-app-client.xlsx
+++ b/src/main/webapp/WEB-INF/books/vendor-app-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipsedata\Workspace\dev-ref-vendor\src\main\webapp\WEB-INF\book\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA45816-CE08-4E70-BB32-4AB6F76B095C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3AABFA-5539-AC42-9AEC-B088B9A45CD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form" sheetId="1" r:id="rId1"/>
@@ -362,7 +362,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -371,38 +378,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,66 +730,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:P79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:M6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53:K56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="3" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="6.125" customWidth="1"/>
-    <col min="5" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="2.625" customWidth="1"/>
-    <col min="7" max="7" width="14.875" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
     <col min="8" max="8" width="3" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="4.375" customWidth="1"/>
-    <col min="11" max="13" width="16.875" customWidth="1"/>
-    <col min="14" max="14" width="3.625" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" customWidth="1"/>
+    <col min="11" max="13" width="16.83203125" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:15" ht="23" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
       <c r="N2" s="4"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:15" ht="23" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+    <row r="4" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -793,7 +803,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -808,7 +818,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -825,7 +835,7 @@
       <c r="N6" s="3"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -840,7 +850,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
@@ -857,7 +867,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -872,7 +882,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
@@ -889,7 +899,7 @@
       <c r="N10" s="3"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -904,7 +914,7 @@
       <c r="N11" s="3"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
@@ -921,7 +931,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -936,7 +946,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
@@ -953,7 +963,7 @@
       <c r="N14" s="3"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -968,7 +978,7 @@
       <c r="N15" s="3"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
@@ -985,7 +995,7 @@
       <c r="N16" s="3"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1000,7 +1010,7 @@
       <c r="N17" s="3"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1013,7 +1023,7 @@
       <c r="N18" s="3"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="3"/>
@@ -1028,11 +1038,11 @@
       <c r="N19" s="3"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
+    <row r="20" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1046,7 +1056,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="2:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:15" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="2"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1061,16 +1071,16 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="10"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -1082,7 +1092,7 @@
       <c r="N22" s="3"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C23" s="1"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1097,16 +1107,16 @@
       <c r="N23" s="3"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="10"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -1118,7 +1128,7 @@
       <c r="N24" s="3"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C25" s="1"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1133,16 +1143,16 @@
       <c r="N25" s="3"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="10"/>
+      <c r="G26" s="12"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
@@ -1154,7 +1164,7 @@
       <c r="N26" s="3"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C27" s="1"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1169,7 +1179,7 @@
       <c r="N27" s="3"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="3"/>
@@ -1184,11 +1194,11 @@
       <c r="N28" s="3"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="2:15" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+    <row r="29" spans="2:15" ht="20" x14ac:dyDescent="0.2">
+      <c r="B29" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="13"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1202,7 +1212,7 @@
       <c r="N29" s="3"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1217,7 +1227,7 @@
       <c r="N30" s="3"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
         <v>20</v>
       </c>
@@ -1236,7 +1246,7 @@
       <c r="N31" s="3"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C32" s="1"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -1251,7 +1261,7 @@
       <c r="N32" s="3"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
         <v>21</v>
       </c>
@@ -1270,7 +1280,7 @@
       <c r="N33" s="3"/>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1285,7 +1295,7 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
         <v>22</v>
       </c>
@@ -1303,7 +1313,7 @@
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1318,7 +1328,7 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1333,7 +1343,7 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="2:16" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:16" ht="20" x14ac:dyDescent="0.2">
       <c r="B38" s="8" t="s">
         <v>41</v>
       </c>
@@ -1351,7 +1361,7 @@
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" s="2"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1366,16 +1376,16 @@
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="10"/>
+      <c r="G40" s="12"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
@@ -1387,7 +1397,7 @@
       <c r="N40" s="3"/>
       <c r="O40" s="1"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C41" s="1"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -1402,16 +1412,16 @@
       <c r="N41" s="3"/>
       <c r="O41" s="1"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C42" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G42" s="10"/>
+      <c r="G42" s="12"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
@@ -1423,7 +1433,7 @@
       <c r="N42" s="3"/>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C43" s="1"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -1438,16 +1448,16 @@
       <c r="N43" s="3"/>
       <c r="O43" s="1"/>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C44" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="10"/>
+      <c r="G44" s="12"/>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
@@ -1459,7 +1469,7 @@
       <c r="N44" s="3"/>
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -1474,9 +1484,9 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="2:16" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
+    <row r="46" spans="2:16" ht="20" x14ac:dyDescent="0.2">
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -1490,11 +1500,11 @@
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="2:16" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B47" s="11" t="s">
+    <row r="47" spans="2:16" ht="20" x14ac:dyDescent="0.2">
+      <c r="B47" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="11"/>
+      <c r="C47" s="13"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -1508,7 +1518,7 @@
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
     </row>
-    <row r="48" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C48" s="2"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -1523,14 +1533,14 @@
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
     </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C49" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
       <c r="H49" s="1" t="s">
         <v>38</v>
       </c>
@@ -1542,7 +1552,7 @@
       <c r="N49" s="3"/>
       <c r="O49" s="1"/>
     </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C50" s="1"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -1557,14 +1567,14 @@
       <c r="N50" s="3"/>
       <c r="O50" s="1"/>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
       <c r="H51" s="5" t="s">
         <v>37</v>
       </c>
@@ -1578,7 +1588,7 @@
       <c r="N51" s="3"/>
       <c r="O51" s="1"/>
     </row>
-    <row r="52" spans="3:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -1593,7 +1603,7 @@
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="14" t="s">
@@ -1610,7 +1620,7 @@
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
     </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:15" x14ac:dyDescent="0.2">
       <c r="E54" s="17"/>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
@@ -1619,7 +1629,7 @@
       <c r="J54" s="18"/>
       <c r="K54" s="19"/>
     </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:15" x14ac:dyDescent="0.2">
       <c r="E55" s="17"/>
       <c r="F55" s="18"/>
       <c r="G55" s="18"/>
@@ -1628,7 +1638,7 @@
       <c r="J55" s="18"/>
       <c r="K55" s="19"/>
     </row>
-    <row r="56" spans="3:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E56" s="20"/>
       <c r="F56" s="21"/>
       <c r="G56" s="21"/>
@@ -1637,18 +1647,51 @@
       <c r="J56" s="21"/>
       <c r="K56" s="22"/>
     </row>
-    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:15" x14ac:dyDescent="0.2">
       <c r="G63" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I79" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="48">
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="G35:M35"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="D8:M8"/>
+    <mergeCell ref="D12:M12"/>
+    <mergeCell ref="D14:M14"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="H26:J26"/>
     <mergeCell ref="E53:K56"/>
     <mergeCell ref="H22:J22"/>
     <mergeCell ref="D18:G18"/>
@@ -1665,38 +1708,6 @@
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="D6:M6"/>
-    <mergeCell ref="D8:M8"/>
-    <mergeCell ref="D12:M12"/>
-    <mergeCell ref="D14:M14"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="G35:M35"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:J44"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D31:E31 D33:E33" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -1719,63 +1730,63 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1793,29 +1804,29 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
fix named range typo
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/vendor-app-client.xlsx
+++ b/src/main/webapp/WEB-INF/books/vendor-app-client.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3AABFA-5539-AC42-9AEC-B088B9A45CD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC0EC7D-24CE-5849-97EE-39D5A7C3971F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <definedName name="businessCategory2">Form!$D$33</definedName>
     <definedName name="businessProductsAndServices">Form!$G$35</definedName>
     <definedName name="Categories">Category!$A$1:$A$11</definedName>
+    <definedName name="companyAddress">Form!$D$8</definedName>
     <definedName name="companyAdress">Form!$D$8</definedName>
     <definedName name="companyName">Form!$D$6</definedName>
     <definedName name="contact1Designation">Form!$I$22</definedName>
@@ -362,22 +363,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -413,6 +398,22 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:P79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53:K56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -750,46 +751,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
       <c r="N2" s="4"/>
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="2:15" ht="23" x14ac:dyDescent="0.2">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -822,16 +823,16 @@
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
       <c r="N6" s="3"/>
       <c r="O6" s="1"/>
     </row>
@@ -854,16 +855,16 @@
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
       <c r="N8" s="3"/>
       <c r="O8" s="1"/>
     </row>
@@ -886,16 +887,16 @@
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
       <c r="N10" s="3"/>
       <c r="O10" s="1"/>
     </row>
@@ -918,16 +919,16 @@
       <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
       <c r="N12" s="3"/>
       <c r="O12" s="1"/>
     </row>
@@ -950,16 +951,16 @@
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
       <c r="N14" s="3"/>
       <c r="O14" s="1"/>
     </row>
@@ -982,16 +983,16 @@
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
       <c r="N16" s="3"/>
       <c r="O16" s="1"/>
     </row>
@@ -1014,12 +1015,12 @@
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
       <c r="N18" s="3"/>
       <c r="O18" s="1"/>
     </row>
@@ -1039,10 +1040,10 @@
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1075,20 +1076,20 @@
       <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="12" t="s">
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
       <c r="K22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
       <c r="N22" s="3"/>
       <c r="O22" s="1"/>
     </row>
@@ -1111,20 +1112,20 @@
       <c r="C24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="12" t="s">
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
       <c r="K24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
       <c r="N24" s="3"/>
       <c r="O24" s="1"/>
     </row>
@@ -1147,20 +1148,20 @@
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="12" t="s">
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
       <c r="K26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
       <c r="N26" s="3"/>
       <c r="O26" s="1"/>
     </row>
@@ -1195,10 +1196,10 @@
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="2:15" ht="20" x14ac:dyDescent="0.2">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1231,12 +1232,12 @@
       <c r="C31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1265,12 +1266,12 @@
       <c r="C33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1302,13 +1303,13 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
@@ -1380,20 +1381,20 @@
       <c r="C40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="12" t="s">
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="12"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
       <c r="K40" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
       <c r="N40" s="3"/>
       <c r="O40" s="1"/>
     </row>
@@ -1416,20 +1417,20 @@
       <c r="C42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="12" t="s">
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G42" s="12"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
       <c r="K42" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
       <c r="N42" s="3"/>
       <c r="O42" s="1"/>
     </row>
@@ -1452,20 +1453,20 @@
       <c r="C44" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="12" t="s">
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="12"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
       <c r="K44" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
       <c r="N44" s="3"/>
       <c r="O44" s="1"/>
     </row>
@@ -1485,8 +1486,8 @@
       <c r="O45" s="1"/>
     </row>
     <row r="46" spans="2:16" ht="20" x14ac:dyDescent="0.2">
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -1501,10 +1502,10 @@
       <c r="O46" s="1"/>
     </row>
     <row r="47" spans="2:16" ht="20" x14ac:dyDescent="0.2">
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="13"/>
+      <c r="C47" s="22"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -1537,17 +1538,17 @@
       <c r="C49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
       <c r="H49" s="1" t="s">
         <v>38</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
-      <c r="K49" s="9"/>
-      <c r="L49" s="9"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
       <c r="M49" s="5"/>
       <c r="N49" s="3"/>
       <c r="O49" s="1"/>
@@ -1571,19 +1572,19 @@
       <c r="C51" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
       <c r="H51" s="5" t="s">
         <v>37</v>
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
-      <c r="K51" s="9" t="s">
+      <c r="K51" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L51" s="9"/>
+      <c r="L51" s="18"/>
       <c r="M51" s="5"/>
       <c r="N51" s="3"/>
       <c r="O51" s="1"/>
@@ -1606,46 +1607,46 @@
     <row r="53" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="16"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="11"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
     </row>
     <row r="54" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E54" s="17"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="19"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="14"/>
     </row>
     <row r="55" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E55" s="17"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="19"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="14"/>
     </row>
     <row r="56" spans="3:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E56" s="20"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="22"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="17"/>
     </row>
     <row r="63" spans="3:15" x14ac:dyDescent="0.2">
       <c r="G63" t="s">
@@ -1710,10 +1711,10 @@
     <mergeCell ref="D6:M6"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D31:E31 D33:E33" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D31:G31 D33:G33" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Categories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18" xr:uid="{95CC3272-EBC3-4A1C-A9EF-FF477F59E58B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18:G18" xr:uid="{95CC3272-EBC3-4A1C-A9EF-FF477F59E58B}">
       <formula1>Legal</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>